<commit_message>
using FIFA algo for team balance and using seperate JSON file for player stats
</commit_message>
<xml_diff>
--- a/Team_Distribution.xlsx
+++ b/Team_Distribution.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Amritpal (C)</t>
+          <t>Jaiswal (C)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -484,60 +484,100 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>shailesh C (MID)</t>
+          <t>nuhu (MID)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dheeraj (MID)</t>
+          <t>ketan (GK)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kartik (MID)</t>
+          <t>shailesh C (MID)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sagar (MID)</t>
+          <t>Jithu (GK)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>abhijit (DEF)</t>
+          <t>Vignesh (MID)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sudeep (DEF)</t>
+          <t>Sagar (MID)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>vishnu (DEF)</t>
+          <t>Bhupinder (MID)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>shailesh (DEF)</t>
+          <t>Amritpal (MID)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>abhijit (DEF)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Kartik (MID)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Saurab (DEF)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DJ (DEF)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>Deepak (DEF)</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Saurab (DEF)</t>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>shailesh (DEF)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Debashish (DEF)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Summet (WS)</t>
         </is>
       </c>
     </row>

</xml_diff>